<commit_message>
added analyses for revision
</commit_message>
<xml_diff>
--- a/data/venom_annotation/fullVenomAnnotation_02.20.20.xlsx
+++ b/data/venom_annotation/fullVenomAnnotation_02.20.20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/perryb/Dropbox/CastoeLabFolder/projects/CVV_Gene_Regulation/_VenomGeneRegulation/data/venom_annotations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blairperry/Dropbox/CastoeLabFolder/projects/CVV_Gene_Regulation/_VenomGeneRegulation_NEW_Aug2021/data/venom_annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB084A4-4ED4-0749-83A8-0224738872FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54E4895-879C-2144-96B1-1A442EBDDE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24680" yWindow="8500" windowWidth="22840" windowHeight="20120" xr2:uid="{1D3EC956-8218-4146-AF31-8A7C4D30CDD5}"/>
   </bookViews>
@@ -702,7 +702,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -713,6 +713,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -738,9 +745,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1068,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C33C76-AB93-9342-96F8-B766CD3DB563}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1920,22 +1928,22 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>289328153</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="2">
         <v>289328605</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>